<commit_message>
- (WIP) Work on report - Added data comparison spreadsheet
</commit_message>
<xml_diff>
--- a/ds1/ds1_stats.xlsx
+++ b/ds1/ds1_stats.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\soen472_mp2\Data set release 1\ds1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\soen472_mp2\ds1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CF3824-DCFC-477D-8A54-27B4210E4A67}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1585AE-C944-48DE-9B23-9D023A909DB0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" activeTab="2" xr2:uid="{E3F65C83-32B3-4C7A-966E-A0762FD703F3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" activeTab="3" xr2:uid="{E3F65C83-32B3-4C7A-966E-A0762FD703F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
     <sheet name="Validation" sheetId="3" r:id="rId2"/>
     <sheet name="Experimentation" sheetId="4" r:id="rId3"/>
     <sheet name="Adjusted" sheetId="5" r:id="rId4"/>
-    <sheet name="Testing" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>Algorithm</t>
   </si>
@@ -232,6 +231,15 @@
   </si>
   <si>
     <t>Better at 0.2</t>
+  </si>
+  <si>
+    <t>Multilayer Perceptron</t>
+  </si>
+  <si>
+    <t>Multilayer Perceptron (10 epochs / 537 hidden nodes)</t>
+  </si>
+  <si>
+    <t>decay = true</t>
   </si>
 </sst>
 </file>
@@ -314,11 +322,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C695380-AF5B-45A7-BF2D-28CA00309EBE}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -755,18 +763,35 @@
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="D7">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>0.95199999999999996</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>0.95399999999999996</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>0.95199999999999996</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>0.95199999999999996</v>
       </c>
     </row>
@@ -781,7 +806,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E1:E7"/>
+      <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -878,7 +903,19 @@
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="C6">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="D6">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="E6">
+        <v>0.58399999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -899,13 +936,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -920,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7A6426-F1A3-479C-A068-38DE87B162FB}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,7 +1198,7 @@
       <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D20" t="s">
@@ -1281,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BB33D6-6C10-4352-926A-B786B339F69C}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1352,9 +1389,24 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>66</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="D4">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1367,74 +1419,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B99671A-CE46-469F-9F70-DE3054D56DC1}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="27.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>